<commit_message>
Jan 21 - Cart Lang input
</commit_message>
<xml_diff>
--- a/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
+++ b/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Git\gr\gr\Input_Output\CartLanguagePriceValidation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDF8982-86C5-40AA-8FD3-DC77435297C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7724F738-A456-41BE-91DE-4B8FA480BAF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="55">
   <si>
     <t>Environment</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>deluxe25offp-holiday</t>
+  </si>
+  <si>
+    <t>deluxe25off</t>
   </si>
 </sst>
 </file>
@@ -575,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +615,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -626,6 +629,380 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Jan 22 - Input updates
</commit_message>
<xml_diff>
--- a/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
+++ b/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Git\gr\gr\Input_Output\CartLanguagePriceValidation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7724F738-A456-41BE-91DE-4B8FA480BAF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78423CCF-4B1E-458D-A548-0BE7A7D0F19D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="55">
   <si>
     <t>Environment</t>
   </si>
@@ -578,11 +578,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -615,9 +613,9 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
@@ -632,10 +630,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -649,10 +647,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -666,7 +664,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -683,10 +681,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -700,10 +698,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -717,10 +715,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -737,7 +735,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -754,7 +752,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -768,10 +766,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -785,10 +783,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -802,10 +800,10 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -819,10 +817,10 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -836,10 +834,10 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -856,7 +854,7 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -873,7 +871,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -890,7 +888,7 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -904,10 +902,10 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -921,10 +919,10 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -938,10 +936,10 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -952,57 +950,6 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feb 2 - Cart Language Test Data update
</commit_message>
<xml_diff>
--- a/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
+++ b/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Git\gr\gr\Input_Output\CartLanguagePriceValidation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78423CCF-4B1E-458D-A548-0BE7A7D0F19D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB192C06-FBC5-46DC-9349-C4E7692E7A0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="55">
   <si>
     <t>Environment</t>
   </si>
@@ -578,7 +578,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -701,7 +701,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -715,10 +715,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -732,10 +732,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -749,10 +749,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -766,10 +766,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -783,10 +783,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -803,7 +803,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -820,7 +820,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -834,10 +834,10 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -851,10 +851,10 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -868,10 +868,10 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -882,74 +882,6 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
June 15 - Inputs update
</commit_message>
<xml_diff>
--- a/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
+++ b/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\happy\git\gr\gr\Input_Output\CartLanguagePriceValidation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399289B4-B3B1-4948-88DC-AAA3F52E1483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CBA229-5762-4603-B74B-16F0DEBC11B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="57">
   <si>
     <t>Environment</t>
   </si>
@@ -198,7 +198,10 @@
     <t>deluxe25offp-redes</t>
   </si>
   <si>
-    <t>deluxe25offp-redes-spring</t>
+    <t>deluxe25offp-redes-summera</t>
+  </si>
+  <si>
+    <t>deluxe25offp-redes-summerb</t>
   </si>
 </sst>
 </file>
@@ -581,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,7 +861,7 @@
       <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>55</v>
       </c>
       <c r="D16" t="s">
@@ -870,41 +873,41 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -915,7 +918,7 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -929,10 +932,10 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -946,7 +949,7 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
@@ -963,7 +966,7 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
@@ -983,7 +986,7 @@
         <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
@@ -997,10 +1000,10 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -1017,7 +1020,7 @@
         <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
@@ -1034,7 +1037,7 @@
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
@@ -1051,7 +1054,7 @@
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -1068,7 +1071,7 @@
         <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
@@ -1082,10 +1085,10 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
@@ -1102,7 +1105,7 @@
         <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
@@ -1119,7 +1122,7 @@
         <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -1130,6 +1133,23 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
July 16 - email password update and run inputs update
</commit_message>
<xml_diff>
--- a/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
+++ b/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\happy\git\gr\gr\Input_Output\CartLanguagePriceValidation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Code\gr-master\gr\Input_Output\CartLanguagePriceValidation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CBA229-5762-4603-B74B-16F0DEBC11B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80D44E1-3FC7-465C-AEBC-B27C0133E21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="58">
   <si>
     <t>Environment</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>deluxe25offp-redes-summerb</t>
+  </si>
+  <si>
+    <t>deluxe25offp-redes-July4</t>
   </si>
 </sst>
 </file>
@@ -584,22 +587,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.08984375" customWidth="1"/>
+    <col min="3" max="3" width="30.90625" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -633,7 +636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -650,7 +653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -667,7 +670,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -684,7 +687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -701,100 +704,100 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -803,7 +806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -811,200 +814,200 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C33" t="s">
         <v>54</v>
       </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" t="s">
-        <v>22</v>
-      </c>
       <c r="D33" t="s">
         <v>7</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1020,7 +1023,7 @@
         <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
@@ -1029,7 +1032,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1037,7 +1040,7 @@
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
@@ -1046,15 +1049,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -1063,15 +1066,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
@@ -1080,15 +1083,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
@@ -1097,59 +1100,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1176,15 +1128,15 @@
       <selection activeCell="A36" sqref="A36:E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" customWidth="1"/>
+    <col min="3" max="3" width="33.90625" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1218,7 +1170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1235,7 +1187,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1252,7 +1204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1269,7 +1221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1286,7 +1238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1303,7 +1255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1320,7 +1272,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1337,7 +1289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1354,7 +1306,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1371,7 +1323,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1388,7 +1340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1405,7 +1357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1422,7 +1374,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1439,7 +1391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1456,7 +1408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1473,7 +1425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1490,7 +1442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1507,7 +1459,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1524,7 +1476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1541,7 +1493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1558,7 +1510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1575,7 +1527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1592,7 +1544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1609,7 +1561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1626,12 +1578,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1648,7 +1600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1665,7 +1617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1682,7 +1634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1699,7 +1651,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1716,7 +1668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1733,7 +1685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1750,7 +1702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -1767,7 +1719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1784,7 +1736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1801,7 +1753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -1818,7 +1770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -1835,7 +1787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1852,7 +1804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>32</v>
       </c>
@@ -1873,16 +1825,16 @@
       <selection activeCell="A22" sqref="A22:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" customWidth="1"/>
+    <col min="3" max="3" width="24.08984375" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1899,7 +1851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1916,7 +1868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1933,7 +1885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1950,7 +1902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1967,7 +1919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1984,7 +1936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2001,7 +1953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2018,7 +1970,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2035,7 +1987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2052,7 +2004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2069,7 +2021,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2086,7 +2038,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -2103,7 +2055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2120,12 +2072,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -2158,16 +2110,16 @@
       <selection sqref="A1:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" customWidth="1"/>
+    <col min="3" max="3" width="26.36328125" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2184,7 +2136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2201,7 +2153,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2218,7 +2170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2235,7 +2187,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2252,7 +2204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2269,7 +2221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2286,7 +2238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2303,7 +2255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2320,7 +2272,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2337,7 +2289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2354,7 +2306,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2371,7 +2323,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -2388,7 +2340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2405,7 +2357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2422,7 +2374,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -2439,7 +2391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -2456,7 +2408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -2473,7 +2425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -2490,7 +2442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -2507,7 +2459,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -2524,7 +2476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -2541,7 +2493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2558,7 +2510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -2575,7 +2527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Updating cart lang and fb pixel test data and updating buyflow output sheet including Status column
</commit_message>
<xml_diff>
--- a/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
+++ b/gr/Input_Output/CartLanguagePriceValidation/cartlang_kittestdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Code\gr-master\gr\Input_Output\CartLanguagePriceValidation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80D44E1-3FC7-465C-AEBC-B27C0133E21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED719E0-9A60-46BE-916D-C4C7DC4D6100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="58">
   <si>
     <t>Environment</t>
   </si>
@@ -198,13 +198,13 @@
     <t>deluxe25offp-redes</t>
   </si>
   <si>
+    <t>deluxe25offp-redes-July4</t>
+  </si>
+  <si>
     <t>deluxe25offp-redes-summera</t>
   </si>
   <si>
     <t>deluxe25offp-redes-summerb</t>
-  </si>
-  <si>
-    <t>deluxe25offp-redes-July4</t>
   </si>
 </sst>
 </file>
@@ -587,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -797,7 +797,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -814,7 +814,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -831,7 +831,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -842,266 +842,74 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
         <v>23</v>
       </c>
-      <c r="C33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="C34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1822,7 +1630,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:E22"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>